<commit_message>
actualizado a julio 2025
</commit_message>
<xml_diff>
--- a/data/precios_monomico.xlsx
+++ b/data/precios_monomico.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="131">
   <si>
     <t>AGENTE</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Precio Monómico USD/MWh 062025</t>
+  </si>
+  <si>
+    <t>Precio Monómico USD/MWh 072025</t>
   </si>
   <si>
     <t>Arboleda</t>
@@ -761,13 +764,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF90"/>
+  <dimension ref="A1:AG90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:33">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -864,13 +867,16 @@
       <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:32">
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C2">
         <v>24.15137379092663</v>
@@ -878,6 +884,9 @@
       <c r="D2">
         <v>24.51510982292954</v>
       </c>
+      <c r="E2">
+        <v>22.18787282316937</v>
+      </c>
       <c r="F2">
         <v>22.73493104422785</v>
       </c>
@@ -896,16 +905,19 @@
       <c r="Z2">
         <v>23.29043907120782</v>
       </c>
+      <c r="AB2">
+        <v>22.21593711099372</v>
+      </c>
       <c r="AE2">
         <v>23.75334249763923</v>
       </c>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:33">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C3">
         <v>40.24125967809161</v>
@@ -997,13 +1009,16 @@
       <c r="AF3">
         <v>32.23915633002744</v>
       </c>
-    </row>
-    <row r="4" spans="1:32">
+      <c r="AG3">
+        <v>32.69964236888325</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C4">
         <v>34.29539189973546</v>
@@ -1095,13 +1110,16 @@
       <c r="AF4">
         <v>46.98993223340691</v>
       </c>
-    </row>
-    <row r="5" spans="1:32">
+      <c r="AG4">
+        <v>46.01428615359652</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K5">
         <v>35.35346362793552</v>
@@ -1161,12 +1179,12 @@
         <v>50.29081405714062</v>
       </c>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:33">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C6">
         <v>33.41502258070991</v>
@@ -1211,12 +1229,12 @@
         <v>31.13442712539274</v>
       </c>
     </row>
-    <row r="7" spans="1:32">
+    <row r="7" spans="1:33">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C7">
         <v>39.73684227681284</v>
@@ -1243,12 +1261,12 @@
         <v>34.91304298095726</v>
       </c>
     </row>
-    <row r="8" spans="1:32">
+    <row r="8" spans="1:33">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C8">
         <v>31.19813758932338</v>
@@ -1340,13 +1358,16 @@
       <c r="AF8">
         <v>36.81526479786887</v>
       </c>
-    </row>
-    <row r="9" spans="1:32">
+      <c r="AG8">
+        <v>39.09175559638076</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="Y9">
         <v>29.68539184231521</v>
@@ -1372,13 +1393,16 @@
       <c r="AF9">
         <v>29.06896263758356</v>
       </c>
-    </row>
-    <row r="10" spans="1:32">
+      <c r="AG9">
+        <v>29.59363877298952</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G10">
         <v>34.46099289333294</v>
@@ -1455,13 +1479,16 @@
       <c r="AF10">
         <v>50.33124569641992</v>
       </c>
-    </row>
-    <row r="11" spans="1:32">
+      <c r="AG10">
+        <v>53.84140745150569</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C11">
         <v>24.53315654997625</v>
@@ -1553,13 +1580,16 @@
       <c r="AF11">
         <v>27.85764788230211</v>
       </c>
-    </row>
-    <row r="12" spans="1:32">
+      <c r="AG11">
+        <v>25.74935834872135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C12">
         <v>34.55886279192773</v>
@@ -1651,13 +1681,16 @@
       <c r="AF12">
         <v>45.98970522505112</v>
       </c>
-    </row>
-    <row r="13" spans="1:32">
+      <c r="AG12">
+        <v>45.72939257589278</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C13">
         <v>34.78449303993775</v>
@@ -1749,13 +1782,16 @@
       <c r="AF13">
         <v>41.9008935665164</v>
       </c>
-    </row>
-    <row r="14" spans="1:32">
+      <c r="AG13">
+        <v>42.56759793084879</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C14">
         <v>32.62190327673912</v>
@@ -1847,13 +1883,16 @@
       <c r="AF14">
         <v>41.64849541191397</v>
       </c>
-    </row>
-    <row r="15" spans="1:32">
+      <c r="AG14">
+        <v>40.3487627846451</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C15">
         <v>38.48737986216626</v>
@@ -1933,13 +1972,16 @@
       <c r="AF15">
         <v>40.39194522321687</v>
       </c>
-    </row>
-    <row r="16" spans="1:32">
+      <c r="AG15">
+        <v>39.8939403662717</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="Y16">
         <v>37.59853181683598</v>
@@ -1965,13 +2007,16 @@
       <c r="AF16">
         <v>37.96158414951147</v>
       </c>
-    </row>
-    <row r="17" spans="1:32">
+      <c r="AG16">
+        <v>38.62154059744302</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C17">
         <v>53.26350873556772</v>
@@ -2036,13 +2081,16 @@
       <c r="AF17">
         <v>28.83428806280632</v>
       </c>
-    </row>
-    <row r="18" spans="1:32">
+      <c r="AG17">
+        <v>30.87664186309867</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C18">
         <v>41.15355653986153</v>
@@ -2116,13 +2164,16 @@
       <c r="AF18">
         <v>40.48234965312189</v>
       </c>
-    </row>
-    <row r="19" spans="1:32">
+      <c r="AG18">
+        <v>39.94072774569639</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K19">
         <v>34.9537877001113</v>
@@ -2143,12 +2194,12 @@
         <v>38.70683120288043</v>
       </c>
     </row>
-    <row r="20" spans="1:32">
+    <row r="20" spans="1:33">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B20" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C20">
         <v>39.9300324634649</v>
@@ -2228,13 +2279,16 @@
       <c r="AF20">
         <v>37.15126377283375</v>
       </c>
-    </row>
-    <row r="21" spans="1:32">
+      <c r="AG20">
+        <v>35.81403927300808</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C21">
         <v>29.60504291522077</v>
@@ -2326,13 +2380,16 @@
       <c r="AF21">
         <v>33.34045440752196</v>
       </c>
-    </row>
-    <row r="22" spans="1:32">
+      <c r="AG21">
+        <v>33.33057628386303</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C22">
         <v>32.1632384740019</v>
@@ -2424,13 +2481,16 @@
       <c r="AF22">
         <v>34.75877990597596</v>
       </c>
-    </row>
-    <row r="23" spans="1:32">
+      <c r="AG22">
+        <v>35.54141817989193</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C23">
         <v>39.65940618883968</v>
@@ -2522,13 +2582,16 @@
       <c r="AF23">
         <v>35.10810766508118</v>
       </c>
-    </row>
-    <row r="24" spans="1:32">
+      <c r="AG23">
+        <v>35.67156119693866</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C24">
         <v>41.33478222235261</v>
@@ -2620,13 +2683,16 @@
       <c r="AF24">
         <v>42.77778657351098</v>
       </c>
-    </row>
-    <row r="25" spans="1:32">
+      <c r="AG24">
+        <v>42.44971592058937</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AE25">
         <v>28.47375654197985</v>
@@ -2634,13 +2700,16 @@
       <c r="AF25">
         <v>27.139695613351</v>
       </c>
-    </row>
-    <row r="26" spans="1:32">
+      <c r="AG25">
+        <v>25.9226597383855</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C26">
         <v>28.07394932990581</v>
@@ -2708,16 +2777,19 @@
       <c r="Y26">
         <v>22.56468047502521</v>
       </c>
+      <c r="Z26">
+        <v>22.1981314334199</v>
+      </c>
       <c r="AE26">
         <v>22.88441913760912</v>
       </c>
     </row>
-    <row r="27" spans="1:32">
+    <row r="27" spans="1:33">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B27" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="Y27">
         <v>36.46511059378976</v>
@@ -2743,13 +2815,16 @@
       <c r="AF27">
         <v>34.05399752883125</v>
       </c>
-    </row>
-    <row r="28" spans="1:32">
+      <c r="AG27">
+        <v>32.9468006919914</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C28">
         <v>31.14100412491597</v>
@@ -2841,13 +2916,16 @@
       <c r="AF28">
         <v>31.21864308293326</v>
       </c>
-    </row>
-    <row r="29" spans="1:32">
+      <c r="AG28">
+        <v>31.88334697491996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C29">
         <v>34.78607129082696</v>
@@ -2927,13 +3005,16 @@
       <c r="AF29">
         <v>38.1671283826546</v>
       </c>
-    </row>
-    <row r="30" spans="1:32">
+      <c r="AG29">
+        <v>36.48672529161526</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C30">
         <v>33.03357756871915</v>
@@ -3025,13 +3106,16 @@
       <c r="AF30">
         <v>43.52690998411664</v>
       </c>
-    </row>
-    <row r="31" spans="1:32">
+      <c r="AG30">
+        <v>43.78542111227741</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C31">
         <v>40.03106481251331</v>
@@ -3069,13 +3153,16 @@
       <c r="AF31">
         <v>36.75323723038639</v>
       </c>
-    </row>
-    <row r="32" spans="1:32">
+      <c r="AG31">
+        <v>37.26742853907398</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C32">
         <v>36.05996037615198</v>
@@ -3125,13 +3212,16 @@
       <c r="AF32">
         <v>25.3667192331101</v>
       </c>
-    </row>
-    <row r="33" spans="1:32">
+      <c r="AG32">
+        <v>27.72593391692779</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C33">
         <v>36.99418406811095</v>
@@ -3223,13 +3313,16 @@
       <c r="AF33">
         <v>38.61320323021625</v>
       </c>
-    </row>
-    <row r="34" spans="1:32">
+      <c r="AG33">
+        <v>39.14873721655561</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B34" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C34">
         <v>29.82980183828264</v>
@@ -3288,19 +3381,25 @@
       <c r="Y34">
         <v>24.14698941838461</v>
       </c>
+      <c r="Z34">
+        <v>22.22426941705632</v>
+      </c>
       <c r="AE34">
         <v>23.35518566805434</v>
       </c>
       <c r="AF34">
         <v>22.71168445564879</v>
       </c>
-    </row>
-    <row r="35" spans="1:32">
+      <c r="AG34">
+        <v>22.9661670555781</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C35">
         <v>40.90733440741675</v>
@@ -3392,13 +3491,16 @@
       <c r="AF35">
         <v>33.72630254068783</v>
       </c>
-    </row>
-    <row r="36" spans="1:32">
+      <c r="AG35">
+        <v>32.23683503067873</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33">
       <c r="A36" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B36" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C36">
         <v>41.57740838964424</v>
@@ -3490,24 +3592,27 @@
       <c r="AF36">
         <v>37.78990378308606</v>
       </c>
-    </row>
-    <row r="37" spans="1:32">
+      <c r="AG36">
+        <v>36.5719837400327</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B37" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C37">
         <v>38.36403464683018</v>
       </c>
     </row>
-    <row r="38" spans="1:32">
+    <row r="38" spans="1:33">
       <c r="A38" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B38" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K38">
         <v>34.3802317572044</v>
@@ -3528,12 +3633,12 @@
         <v>36.34327042973307</v>
       </c>
     </row>
-    <row r="39" spans="1:32">
+    <row r="39" spans="1:33">
       <c r="A39" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D39">
         <v>26.48077844442605</v>
@@ -3604,13 +3709,16 @@
       <c r="AF39">
         <v>38.74632929637565</v>
       </c>
-    </row>
-    <row r="40" spans="1:32">
+      <c r="AG39">
+        <v>39.85394386640926</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B40" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D40">
         <v>40.68847679160487</v>
@@ -3693,13 +3801,16 @@
       <c r="AF40">
         <v>41.55138644605277</v>
       </c>
-    </row>
-    <row r="41" spans="1:32">
+      <c r="AG40">
+        <v>37.2634805328457</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33">
       <c r="A41" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B41" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C41">
         <v>30.80665888926223</v>
@@ -3791,13 +3902,16 @@
       <c r="AF41">
         <v>31.19366061529239</v>
       </c>
-    </row>
-    <row r="42" spans="1:32">
+      <c r="AG41">
+        <v>31.64152463466362</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B42" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C42">
         <v>47.86291402850968</v>
@@ -3889,13 +4003,16 @@
       <c r="AF42">
         <v>43.23635150281842</v>
       </c>
-    </row>
-    <row r="43" spans="1:32">
+      <c r="AG42">
+        <v>43.43434273089668</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33">
       <c r="A43" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B43" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="Y43">
         <v>31.61741524513779</v>
@@ -3916,12 +4033,12 @@
         <v>32.5645550733533</v>
       </c>
     </row>
-    <row r="44" spans="1:32">
+    <row r="44" spans="1:33">
       <c r="A44" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B44" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C44">
         <v>40.00096983927793</v>
@@ -4013,13 +4130,16 @@
       <c r="AF44">
         <v>30.11366847633766</v>
       </c>
-    </row>
-    <row r="45" spans="1:32">
+      <c r="AG44">
+        <v>32.01598663257231</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33">
       <c r="A45" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B45" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C45">
         <v>35.32542844647919</v>
@@ -4111,13 +4231,16 @@
       <c r="AF45">
         <v>39.67038682579454</v>
       </c>
-    </row>
-    <row r="46" spans="1:32">
+      <c r="AG45">
+        <v>37.70413151707297</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33">
       <c r="A46" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B46" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N46">
         <v>43.79601235842351</v>
@@ -4153,12 +4276,12 @@
         <v>41.25409379619437</v>
       </c>
     </row>
-    <row r="47" spans="1:32">
+    <row r="47" spans="1:33">
       <c r="A47" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B47" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C47">
         <v>34.3478828341741</v>
@@ -4250,13 +4373,16 @@
       <c r="AF47">
         <v>32.68499858441294</v>
       </c>
-    </row>
-    <row r="48" spans="1:32">
+      <c r="AG47">
+        <v>33.44820174505215</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33">
       <c r="A48" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B48" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C48">
         <v>37.70592291515717</v>
@@ -4283,12 +4409,12 @@
         <v>35.59696383455866</v>
       </c>
     </row>
-    <row r="49" spans="1:32">
+    <row r="49" spans="1:33">
       <c r="A49" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B49" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C49">
         <v>36.35374106732907</v>
@@ -4315,12 +4441,12 @@
         <v>38.60379709904421</v>
       </c>
     </row>
-    <row r="50" spans="1:32">
+    <row r="50" spans="1:33">
       <c r="A50" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B50" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K50">
         <v>39.33869512981465</v>
@@ -4388,13 +4514,16 @@
       <c r="AF50">
         <v>38.79252879763839</v>
       </c>
-    </row>
-    <row r="51" spans="1:32">
+      <c r="AG50">
+        <v>39.14231758223107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:33">
       <c r="A51" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K51">
         <v>36.19119397037381</v>
@@ -4462,13 +4591,16 @@
       <c r="AF51">
         <v>39.06859055791396</v>
       </c>
-    </row>
-    <row r="52" spans="1:32">
+      <c r="AG51">
+        <v>40.53459857917843</v>
+      </c>
+    </row>
+    <row r="52" spans="1:33">
       <c r="A52" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B52" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C52">
         <v>36.55616341218122</v>
@@ -4548,13 +4680,16 @@
       <c r="AF52">
         <v>36.82193130314196</v>
       </c>
-    </row>
-    <row r="53" spans="1:32">
+      <c r="AG52">
+        <v>36.91161877175995</v>
+      </c>
+    </row>
+    <row r="53" spans="1:33">
       <c r="A53" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B53" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C53">
         <v>33.0354005810775</v>
@@ -4646,13 +4781,16 @@
       <c r="AF53">
         <v>39.1573154995276</v>
       </c>
-    </row>
-    <row r="54" spans="1:32">
+      <c r="AG53">
+        <v>38.27304911061233</v>
+      </c>
+    </row>
+    <row r="54" spans="1:33">
       <c r="A54" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B54" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G54">
         <v>43.25406577131</v>
@@ -4732,13 +4870,16 @@
       <c r="AF54">
         <v>48.01124041314115</v>
       </c>
-    </row>
-    <row r="55" spans="1:32">
+      <c r="AG54">
+        <v>49.18042078463479</v>
+      </c>
+    </row>
+    <row r="55" spans="1:33">
       <c r="A55" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B55" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C55">
         <v>36.21023670628169</v>
@@ -4830,13 +4971,16 @@
       <c r="AF55">
         <v>47.41118942125031</v>
       </c>
-    </row>
-    <row r="56" spans="1:32">
+      <c r="AG55">
+        <v>46.81638740188851</v>
+      </c>
+    </row>
+    <row r="56" spans="1:33">
       <c r="A56" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B56" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C56">
         <v>49.72408892816227</v>
@@ -4928,13 +5072,16 @@
       <c r="AF56">
         <v>41.4643375970406</v>
       </c>
-    </row>
-    <row r="57" spans="1:32">
+      <c r="AG56">
+        <v>40.62402491536265</v>
+      </c>
+    </row>
+    <row r="57" spans="1:33">
       <c r="A57" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B57" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C57">
         <v>36.86413636151038</v>
@@ -5026,13 +5173,16 @@
       <c r="AF57">
         <v>44.42389435466448</v>
       </c>
-    </row>
-    <row r="58" spans="1:32">
+      <c r="AG57">
+        <v>44.08440622193284</v>
+      </c>
+    </row>
+    <row r="58" spans="1:33">
       <c r="A58" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B58" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C58">
         <v>36.0295420612001</v>
@@ -5124,13 +5274,16 @@
       <c r="AF58">
         <v>48.72479383774386</v>
       </c>
-    </row>
-    <row r="59" spans="1:32">
+      <c r="AG58">
+        <v>46.8408312613927</v>
+      </c>
+    </row>
+    <row r="59" spans="1:33">
       <c r="A59" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B59" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C59">
         <v>49.37189062568965</v>
@@ -5219,13 +5372,16 @@
       <c r="AF59">
         <v>37.87412629640171</v>
       </c>
-    </row>
-    <row r="60" spans="1:32">
+      <c r="AG59">
+        <v>36.94934062508471</v>
+      </c>
+    </row>
+    <row r="60" spans="1:33">
       <c r="A60" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B60" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C60">
         <v>37.58314673963842</v>
@@ -5317,13 +5473,16 @@
       <c r="AF60">
         <v>37.59139662434721</v>
       </c>
-    </row>
-    <row r="61" spans="1:32">
+      <c r="AG60">
+        <v>36.28559884941376</v>
+      </c>
+    </row>
+    <row r="61" spans="1:33">
       <c r="A61" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B61" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C61">
         <v>23.26847982742445</v>
@@ -5331,6 +5490,9 @@
       <c r="D61">
         <v>23.13620204779309</v>
       </c>
+      <c r="E61">
+        <v>22.18377284010178</v>
+      </c>
       <c r="G61">
         <v>31.53028914825057</v>
       </c>
@@ -5409,13 +5571,16 @@
       <c r="AF61">
         <v>25.93140534067378</v>
       </c>
-    </row>
-    <row r="62" spans="1:32">
+      <c r="AG61">
+        <v>26.33230892126593</v>
+      </c>
+    </row>
+    <row r="62" spans="1:33">
       <c r="A62" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B62" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C62">
         <v>38.94013284636993</v>
@@ -5489,13 +5654,16 @@
       <c r="AF62">
         <v>40.67890223335612</v>
       </c>
-    </row>
-    <row r="63" spans="1:32">
+      <c r="AG62">
+        <v>40.90235699202768</v>
+      </c>
+    </row>
+    <row r="63" spans="1:33">
       <c r="A63" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B63" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K63">
         <v>40.60077147515437</v>
@@ -5516,12 +5684,12 @@
         <v>41.71276576270834</v>
       </c>
     </row>
-    <row r="64" spans="1:32">
+    <row r="64" spans="1:33">
       <c r="A64" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B64" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C64">
         <v>32.8902103271124</v>
@@ -5580,13 +5748,16 @@
       <c r="AF64">
         <v>45.14711528758943</v>
       </c>
-    </row>
-    <row r="65" spans="1:32">
+      <c r="AG64">
+        <v>46.02424083797317</v>
+      </c>
+    </row>
+    <row r="65" spans="1:33">
       <c r="A65" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B65" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C65">
         <v>39.34198832060151</v>
@@ -5678,13 +5849,16 @@
       <c r="AF65">
         <v>41.43717369954847</v>
       </c>
-    </row>
-    <row r="66" spans="1:32">
+      <c r="AG65">
+        <v>36.64954021233301</v>
+      </c>
+    </row>
+    <row r="66" spans="1:33">
       <c r="A66" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B66" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C66">
         <v>39.24952215971364</v>
@@ -5776,13 +5950,16 @@
       <c r="AF66">
         <v>40.07499043654252</v>
       </c>
-    </row>
-    <row r="67" spans="1:32">
+      <c r="AG66">
+        <v>40.222575918827</v>
+      </c>
+    </row>
+    <row r="67" spans="1:33">
       <c r="A67" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B67" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="M67">
         <v>42.11448249548962</v>
@@ -5832,13 +6009,16 @@
       <c r="AF67">
         <v>30.18904902862487</v>
       </c>
-    </row>
-    <row r="68" spans="1:32">
+      <c r="AG67">
+        <v>33.2994543806436</v>
+      </c>
+    </row>
+    <row r="68" spans="1:33">
       <c r="A68" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B68" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C68">
         <v>46.54448733655986</v>
@@ -5930,13 +6110,16 @@
       <c r="AF68">
         <v>34.91536614398272</v>
       </c>
-    </row>
-    <row r="69" spans="1:32">
+      <c r="AG68">
+        <v>33.03382673957199</v>
+      </c>
+    </row>
+    <row r="69" spans="1:33">
       <c r="A69" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B69" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C69">
         <v>34.32739007240234</v>
@@ -6028,13 +6211,16 @@
       <c r="AF69">
         <v>37.26892113668283</v>
       </c>
-    </row>
-    <row r="70" spans="1:32">
+      <c r="AG69">
+        <v>37.81867010196672</v>
+      </c>
+    </row>
+    <row r="70" spans="1:33">
       <c r="A70" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B70" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C70">
         <v>36.43238580339865</v>
@@ -6126,13 +6312,16 @@
       <c r="AF70">
         <v>37.9833264882649</v>
       </c>
-    </row>
-    <row r="71" spans="1:32">
+      <c r="AG70">
+        <v>37.75784553296767</v>
+      </c>
+    </row>
+    <row r="71" spans="1:33">
       <c r="A71" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B71" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K71">
         <v>36.33086996113984</v>
@@ -6200,13 +6389,16 @@
       <c r="AF71">
         <v>39.64703298379909</v>
       </c>
-    </row>
-    <row r="72" spans="1:32">
+      <c r="AG71">
+        <v>34.5399213189161</v>
+      </c>
+    </row>
+    <row r="72" spans="1:33">
       <c r="A72" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B72" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K72">
         <v>34.76644171888089</v>
@@ -6274,13 +6466,16 @@
       <c r="AF72">
         <v>50.90105871598524</v>
       </c>
-    </row>
-    <row r="73" spans="1:32">
+      <c r="AG72">
+        <v>49.18458460341575</v>
+      </c>
+    </row>
+    <row r="73" spans="1:33">
       <c r="A73" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B73" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C73">
         <v>40.47390929963007</v>
@@ -6307,12 +6502,12 @@
         <v>34.63400714407901</v>
       </c>
     </row>
-    <row r="74" spans="1:32">
+    <row r="74" spans="1:33">
       <c r="A74" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B74" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C74">
         <v>36.36277097879656</v>
@@ -6339,12 +6534,12 @@
         <v>34.72032545196038</v>
       </c>
     </row>
-    <row r="75" spans="1:32">
+    <row r="75" spans="1:33">
       <c r="A75" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B75" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C75">
         <v>40.15830177791462</v>
@@ -6425,12 +6620,12 @@
         <v>45.54196855248671</v>
       </c>
     </row>
-    <row r="76" spans="1:32">
+    <row r="76" spans="1:33">
       <c r="A76" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B76" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C76">
         <v>41.67116846352396</v>
@@ -6475,12 +6670,12 @@
         <v>38.74134350437151</v>
       </c>
     </row>
-    <row r="77" spans="1:32">
+    <row r="77" spans="1:33">
       <c r="A77" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B77" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="Q77">
         <v>36.34951888816632</v>
@@ -6524,13 +6719,16 @@
       <c r="AF77">
         <v>49.40874325886827</v>
       </c>
-    </row>
-    <row r="78" spans="1:32">
+      <c r="AG77">
+        <v>46.74083571266501</v>
+      </c>
+    </row>
+    <row r="78" spans="1:33">
       <c r="A78" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B78" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K78">
         <v>41.03543994350829</v>
@@ -6598,13 +6796,16 @@
       <c r="AF78">
         <v>34.90499147389247</v>
       </c>
-    </row>
-    <row r="79" spans="1:32">
+      <c r="AG78">
+        <v>35.13408724493344</v>
+      </c>
+    </row>
+    <row r="79" spans="1:33">
       <c r="A79" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B79" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C79">
         <v>40.87071757685688</v>
@@ -6631,12 +6832,12 @@
         <v>38.69820317624132</v>
       </c>
     </row>
-    <row r="80" spans="1:32">
+    <row r="80" spans="1:33">
       <c r="A80" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B80" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C80">
         <v>40.3184675932295</v>
@@ -6728,13 +6929,16 @@
       <c r="AF80">
         <v>44.94712927921606</v>
       </c>
-    </row>
-    <row r="81" spans="1:32">
+      <c r="AG80">
+        <v>45.12945735171192</v>
+      </c>
+    </row>
+    <row r="81" spans="1:33">
       <c r="A81" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B81" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C81">
         <v>33.09341370033773</v>
@@ -6826,13 +7030,16 @@
       <c r="AF81">
         <v>45.86525269776246</v>
       </c>
-    </row>
-    <row r="82" spans="1:32">
+      <c r="AG81">
+        <v>44.56927622048666</v>
+      </c>
+    </row>
+    <row r="82" spans="1:33">
       <c r="A82" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B82" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C82">
         <v>32.21630216064776</v>
@@ -6924,13 +7131,16 @@
       <c r="AF82">
         <v>50.23417087057842</v>
       </c>
-    </row>
-    <row r="83" spans="1:32">
+      <c r="AG82">
+        <v>50.16995908811974</v>
+      </c>
+    </row>
+    <row r="83" spans="1:33">
       <c r="A83" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B83" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C83">
         <v>36.61864152099315</v>
@@ -7022,13 +7232,16 @@
       <c r="AF83">
         <v>35.8254458881836</v>
       </c>
-    </row>
-    <row r="84" spans="1:32">
+      <c r="AG83">
+        <v>36.26012053221369</v>
+      </c>
+    </row>
+    <row r="84" spans="1:33">
       <c r="A84" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B84" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I84">
         <v>48.47313294899727</v>
@@ -7060,13 +7273,16 @@
       <c r="AF84">
         <v>37.92963040300597</v>
       </c>
-    </row>
-    <row r="85" spans="1:32">
+      <c r="AG84">
+        <v>38.67013335987262</v>
+      </c>
+    </row>
+    <row r="85" spans="1:33">
       <c r="A85" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B85" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C85">
         <v>32.35697919678239</v>
@@ -7158,13 +7374,16 @@
       <c r="AF85">
         <v>36.33639816128908</v>
       </c>
-    </row>
-    <row r="86" spans="1:32">
+      <c r="AG85">
+        <v>34.82403661884039</v>
+      </c>
+    </row>
+    <row r="86" spans="1:33">
       <c r="A86" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B86" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C86">
         <v>32.36586108796843</v>
@@ -7256,13 +7475,16 @@
       <c r="AF86">
         <v>53.88946085749669</v>
       </c>
-    </row>
-    <row r="87" spans="1:32">
+      <c r="AG86">
+        <v>48.81635211714624</v>
+      </c>
+    </row>
+    <row r="87" spans="1:33">
       <c r="A87" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B87" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C87">
         <v>32.33371854511</v>
@@ -7354,13 +7576,16 @@
       <c r="AF87">
         <v>48.49602182597824</v>
       </c>
-    </row>
-    <row r="88" spans="1:32">
+      <c r="AG87">
+        <v>48.14701806902729</v>
+      </c>
+    </row>
+    <row r="88" spans="1:33">
       <c r="A88" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B88" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K88">
         <v>35.66776913987918</v>
@@ -7381,12 +7606,12 @@
         <v>34.58413080395751</v>
       </c>
     </row>
-    <row r="89" spans="1:32">
+    <row r="89" spans="1:33">
       <c r="A89" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B89" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C89">
         <v>32.24715419253584</v>
@@ -7460,13 +7685,16 @@
       <c r="AF89">
         <v>43.03730922227379</v>
       </c>
-    </row>
-    <row r="90" spans="1:32">
+      <c r="AG89">
+        <v>41.13574080479947</v>
+      </c>
+    </row>
+    <row r="90" spans="1:33">
       <c r="A90" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B90" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C90">
         <v>23.65765560376194</v>
@@ -7557,6 +7785,9 @@
       </c>
       <c r="AF90">
         <v>38.20725144972567</v>
+      </c>
+      <c r="AG90">
+        <v>37.06564795259946</v>
       </c>
     </row>
   </sheetData>

</xml_diff>